<commit_message>
Code updated 23-02-23 15:02:02
</commit_message>
<xml_diff>
--- a/Season_Trophies/84.xlsx
+++ b/Season_Trophies/84.xlsx
@@ -396,7 +396,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>28356</t>
+          <t>25203</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -416,14 +416,14 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>3647</t>
+          <t>3927</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>6</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -443,14 +443,14 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>6369</t>
+          <t>6735</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1526</t>
+          <t>1239</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -470,24 +470,24 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>5841</t>
+          <t>6208</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>4091</t>
+          <t>3639</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>11783968</t>
+          <t>22497</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>F---119</t>
+          <t>xixihahagggᶻᵍˣ</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -497,24 +497,24 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>5398</t>
+          <t>5721</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>4109</t>
+          <t>4444</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>22497</t>
+          <t>11783968</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>xixihahagggᶻᵍˣ</t>
+          <t>F---119</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -524,14 +524,14 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>5395</t>
+          <t>5607</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>5660</t>
+          <t>5266</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -551,14 +551,14 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>5207</t>
+          <t>5495</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>8826</t>
+          <t>7895</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -578,24 +578,24 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>4854</t>
+          <t>5155</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>8824</t>
+          <t>8257</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>43800641</t>
+          <t>21665473</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>㊥蛋蛋大</t>
+          <t>"Dog Gamedesiger"</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -605,24 +605,24 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>4854</t>
+          <t>5114</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>8990</t>
+          <t>9475</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>21665473</t>
+          <t>43800641</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>"Dog Gamedesiger"</t>
+          <t>㊥蛋蛋大</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -632,24 +632,24 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>4838</t>
+          <t>4989</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>714</t>
+          <t>15</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>3946814</t>
+          <t>47928278</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>"小瑩 潘"</t>
+          <t>"落日幻影 哈哈哈"</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -659,24 +659,24 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>6064</t>
+          <t>6706</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>952</t>
+          <t>347</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>31267627</t>
+          <t>3946814</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>"㊥ Martin"</t>
+          <t>"小瑩 潘"</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -686,14 +686,14 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>5994</t>
+          <t>6490</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>958</t>
+          <t>1104</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -713,24 +713,24 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>5992</t>
+          <t>6242</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1250</t>
+          <t>1211</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>47928278</t>
+          <t>31267627</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>"落日幻影 哈哈哈"</t>
+          <t>"㊥ Martin"</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -740,14 +740,14 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>5909</t>
+          <t>6216</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>1306</t>
+          <t>1789</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -767,14 +767,14 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>5896</t>
+          <t>6072</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>1808</t>
+          <t>2103</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -794,24 +794,24 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>5777</t>
+          <t>5998</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2470</t>
+          <t>2488</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>46422609</t>
+          <t>25376635</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>㊥林天大大神</t>
+          <t>"sanchez ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -821,24 +821,24 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>5640</t>
+          <t>5918</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2715</t>
+          <t>2996</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>21735478</t>
+          <t>46422609</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>耀翔fly</t>
+          <t>㊥林天大大神</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -848,24 +848,24 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>5597</t>
+          <t>5819</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2979</t>
+          <t>2949</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>26588375</t>
+          <t>29211638</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>kusipao</t>
+          <t>"㊥ PhononDisperse"</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -875,24 +875,24 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>5555</t>
+          <t>5828</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2991</t>
+          <t>3194</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>29211638</t>
+          <t>21735478</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>"㊥ PhononDisperse"</t>
+          <t>耀翔fly</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -902,24 +902,24 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>5553</t>
+          <t>5788</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>3659</t>
+          <t>3606</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>25376635</t>
+          <t>24733875</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>"sanchez ᶻᵍˣ"</t>
+          <t>龍少</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -929,24 +929,24 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>5455</t>
+          <t>5725</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>3779</t>
+          <t>3803</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>38711610</t>
+          <t>33656016</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>心灵有为</t>
+          <t>㊥☆梅海听雪☆</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -956,24 +956,24 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>5437</t>
+          <t>5695</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>3997</t>
+          <t>4170</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>33656016</t>
+          <t>26588375</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>㊥☆梅海听雪☆</t>
+          <t>kusipao</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -983,24 +983,24 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>5408</t>
+          <t>5642</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>4628</t>
+          <t>4387</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>24733875</t>
+          <t>3477306</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>龍少</t>
+          <t>"MeGa Tsai"</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1010,24 +1010,24 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>5329</t>
+          <t>5614</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>5030</t>
+          <t>4427</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>28387448</t>
+          <t>38711610</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>☜⊙‖⊙☞</t>
+          <t>心灵有为</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1037,24 +1037,24 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>5281</t>
+          <t>5609</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>5259</t>
+          <t>5378</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>3477306</t>
+          <t>28387448</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>"MeGa Tsai"</t>
+          <t>☜⊙‖⊙☞</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1064,24 +1064,24 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>5254</t>
+          <t>5482</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>5359</t>
+          <t>5535</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>29729468</t>
+          <t>9541747</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>"风神舞动 WDᶻᵍˣ"</t>
+          <t>豹子头林冲</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1091,24 +1091,24 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>5243</t>
+          <t>5461</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>5885</t>
+          <t>5866</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>26280580</t>
+          <t>29729468</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>꧁S.TIGRESS꧂ᶻᵍˣ</t>
+          <t>"风神舞动 WDᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1118,24 +1118,24 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>5180</t>
+          <t>5417</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>5929</t>
+          <t>6333</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>9541747</t>
+          <t>30411791</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>豹子头林冲</t>
+          <t>"㊥Ⓩ GOÐAFRÆÐI ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1145,24 +1145,24 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>5173</t>
+          <t>5359</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>6598</t>
+          <t>6362</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>30411791</t>
+          <t>1951758</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>"㊥Ⓩ GOÐAFRÆÐI ᶻᵍˣ"</t>
+          <t>我來找你了</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1172,24 +1172,24 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>5090</t>
+          <t>5355</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>7109</t>
+          <t>6831</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>1951758</t>
+          <t>6510348</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>我來找你了</t>
+          <t>Bonpoisson</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1199,24 +1199,24 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>5029</t>
+          <t>5292</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>7826</t>
+          <t>7442</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>21345373</t>
+          <t>7025661</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>林北不講武德</t>
+          <t>"F ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1226,24 +1226,24 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>4954</t>
+          <t>5211</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>8481</t>
+          <t>7518</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>6510348</t>
+          <t>21345373</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Bonpoisson</t>
+          <t>林北不講武德</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1253,24 +1253,24 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>4888</t>
+          <t>5203</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>8771</t>
+          <t>7911</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>4229136</t>
+          <t>26280580</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>"totoro wu"</t>
+          <t>꧁S.TIGRESS꧂ᶻᵍˣ</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1280,24 +1280,24 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>4859</t>
+          <t>5153</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>9117</t>
+          <t>8068</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>7025661</t>
+          <t>44955827</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>"F ᶻᵍˣ"</t>
+          <t>丶小阿狸丿</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1307,24 +1307,24 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>4826</t>
+          <t>5135</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>11466</t>
+          <t>9839</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>44955827</t>
+          <t>4229136</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>丶小阿狸丿</t>
+          <t>"totoro wu"</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1334,24 +1334,24 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>4633</t>
+          <t>4956</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>14432</t>
+          <t>9914</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>12333251</t>
+          <t>20737010</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>"㊌ Mingxuan"</t>
+          <t>混着玩...</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1361,24 +1361,24 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>4409</t>
+          <t>4950</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>14577</t>
+          <t>13355</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>29861826</t>
+          <t>47146736</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>★★★Eric★★★</t>
+          <t>"HK 品瑜"</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1388,24 +1388,24 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>4400</t>
+          <t>4660</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>14921</t>
+          <t>15321</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>20737010</t>
+          <t>29861826</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>混着玩...</t>
+          <t>★★★Eric★★★</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1415,24 +1415,24 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>4374</t>
+          <t>4509</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>16408</t>
+          <t>16695</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>14424176</t>
+          <t>12333251</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>天才少年老纪</t>
+          <t>"㊌ Mingxuan"</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1442,24 +1442,24 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>4274</t>
+          <t>4419</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>16870</t>
+          <t>16672</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>47146736</t>
+          <t>14424176</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>"HK 品瑜"</t>
+          <t>天才少年老纪</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1469,14 +1469,14 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>4247</t>
+          <t>4420</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>35066</t>
+          <t>32740</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1496,24 +1496,24 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>3369</t>
+          <t>3570</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>46657</t>
+          <t>41497</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>7587898</t>
+          <t>45967307</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>藍精靈ᶻᵍˣ</t>
+          <t>Ricky</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1523,24 +1523,24 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2914</t>
+          <t>3199</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>47910</t>
+          <t>48195</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>45967307</t>
+          <t>7587898</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Ricky</t>
+          <t>藍精靈ᶻᵍˣ</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1550,7 +1550,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2870</t>
+          <t>2914</t>
         </is>
       </c>
     </row>
@@ -1584,7 +1584,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>17266</t>
+          <t>17608</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1604,14 +1604,14 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>4224</t>
+          <t>4364</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>17169</t>
+          <t>17815</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1631,14 +1631,14 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>4230</t>
+          <t>4350</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>8101</t>
+          <t>7521</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1658,14 +1658,14 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>4928</t>
+          <t>5203</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>8724</t>
+          <t>8618</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1685,14 +1685,14 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>4864</t>
+          <t>5072</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>9210</t>
+          <t>9410</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1712,14 +1712,14 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>4820</t>
+          <t>4994</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>10972</t>
+          <t>10420</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1739,14 +1739,14 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>4670</t>
+          <t>4901</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>13383</t>
+          <t>14139</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1766,14 +1766,14 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>4485</t>
+          <t>4596</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>16338</t>
+          <t>16178</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1793,24 +1793,24 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>4278</t>
+          <t>4452</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>16425</t>
+          <t>16777</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>31495601</t>
+          <t>4756174</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>陈晓军</t>
+          <t>純希です</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1820,24 +1820,24 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>4273</t>
+          <t>4414</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>18759</t>
+          <t>19044</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>4756174</t>
+          <t>31495601</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>純希です</t>
+          <t>陈晓军</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1847,14 +1847,14 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>4144</t>
+          <t>4280</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>26907</t>
+          <t>31232</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1874,14 +1874,14 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>3713</t>
+          <t>3638</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>34729</t>
+          <t>37036</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1908,7 +1908,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>256</t>
+          <t>356</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1928,14 +1928,14 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>6242</t>
+          <t>6485</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>593</t>
+          <t>904</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1955,24 +1955,24 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>6103</t>
+          <t>6301</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>4382</t>
+          <t>3243</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>4493731</t>
+          <t>16206490</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Player-1527362</t>
+          <t>㊥Godcys</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1982,24 +1982,24 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>5357</t>
+          <t>5783</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>5686</t>
+          <t>5072</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>16206490</t>
+          <t>4493731</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>㊥Godcys</t>
+          <t>Player-1527362</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2009,14 +2009,14 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>5205</t>
+          <t>5521</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>5739</t>
+          <t>5699</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -2036,14 +2036,14 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>5197</t>
+          <t>5439</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6976</t>
+          <t>7244</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -2063,24 +2063,24 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>5043</t>
+          <t>5236</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>8927</t>
+          <t>8609</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>47131129</t>
+          <t>27484940</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>NAM</t>
+          <t>66666zgx</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -2090,24 +2090,24 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>4843</t>
+          <t>5074</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>9192</t>
+          <t>9011</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>27484940</t>
+          <t>47131129</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>66666zgx</t>
+          <t>NAM</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2117,24 +2117,24 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>4821</t>
+          <t>5030</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>10126</t>
+          <t>10147</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>22885399</t>
+          <t>11582001</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>余文琪</t>
+          <t>iMinatoX4</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2144,24 +2144,24 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>4741</t>
+          <t>4930</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>11758</t>
+          <t>11276</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>11582001</t>
+          <t>22885399</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>iMinatoX4</t>
+          <t>余文琪</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2171,14 +2171,14 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>4611</t>
+          <t>4829</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>11925</t>
+          <t>13696</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -2198,14 +2198,14 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>4597</t>
+          <t>4632</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>17687</t>
+          <t>16773</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -2225,14 +2225,14 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>4202</t>
+          <t>4414</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>17918</t>
+          <t>17167</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -2252,14 +2252,14 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>4189</t>
+          <t>4391</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>19662</t>
+          <t>21823</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2279,14 +2279,14 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>4092</t>
+          <t>4115</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>28697</t>
+          <t>30989</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2306,14 +2306,14 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>3632</t>
+          <t>3648</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>31403</t>
+          <t>33987</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2333,14 +2333,14 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>3518</t>
+          <t>3515</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>32723</t>
+          <t>35018</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -2360,14 +2360,14 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>3462</t>
+          <t>3470</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>36921</t>
+          <t>37341</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2387,14 +2387,14 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>3293</t>
+          <t>3370</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>39840</t>
+          <t>40848</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2414,14 +2414,14 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>3180</t>
+          <t>3226</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>39904</t>
+          <t>41486</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2441,14 +2441,14 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>3177</t>
+          <t>3199</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>42117</t>
+          <t>44052</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2475,7 +2475,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>43667</t>
+          <t>45121</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2495,24 +2495,24 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>3026</t>
+          <t>3041</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>44195</t>
+          <t>45390</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>54714516</t>
+          <t>56500325</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>ёмιいч</t>
+          <t>haruharuyukizg9735</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -2522,24 +2522,24 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>3005</t>
+          <t>3030</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>44744</t>
+          <t>47322</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>56500325</t>
+          <t>54714516</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>haruharuyukizg9735</t>
+          <t>ёмιいч</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -2549,24 +2549,24 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>2986</t>
+          <t>2951</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>48279</t>
+          <t>48922</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>29565</t>
+          <t>1550355</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>"aK.j Zhong ㊥"</t>
+          <t>"皓茵 世界"</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -2576,24 +2576,24 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>2857</t>
+          <t>2889</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>48470</t>
+          <t>49017</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>1550355</t>
+          <t>29565</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>"皓茵 世界"</t>
+          <t>"aK.j Zhong ㊥"</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -2603,24 +2603,24 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>2850</t>
+          <t>2885</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>49321</t>
+          <t>49647</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>58203298</t>
+          <t>68132</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>权旨qua</t>
+          <t>"㊖TW9 百媚生"</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -2630,24 +2630,24 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>2821</t>
+          <t>2860</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>50276</t>
+          <t>49706</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>68132</t>
+          <t>58203298</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>"㊖TW9 百媚生"</t>
+          <t>权旨qua</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -2657,14 +2657,14 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>2789</t>
+          <t>2858</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>50382</t>
+          <t>52190</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2684,14 +2684,14 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>2786</t>
+          <t>2772</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>52164</t>
+          <t>55244</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -2711,14 +2711,14 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>2732</t>
+          <t>2684</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>55494</t>
+          <t>57107</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2738,14 +2738,14 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>2642</t>
+          <t>2634</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>59003</t>
+          <t>60405</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2765,7 +2765,7 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>2567</t>
+          <t>2563</t>
         </is>
       </c>
     </row>
@@ -2826,7 +2826,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>15289</t>
+          <t>16148</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -2846,7 +2846,7 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>4349</t>
+          <t>4454</t>
         </is>
       </c>
     </row>
@@ -2880,7 +2880,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>21370</t>
+          <t>20228</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -2900,24 +2900,24 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>3999</t>
+          <t>4208</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>24035</t>
+          <t>21917</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>25479797</t>
+          <t>54778421</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>"Mohamed Alnaqbi"</t>
+          <t>Emma</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -2927,24 +2927,24 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>3856</t>
+          <t>4110</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>24182</t>
+          <t>25132</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>54778421</t>
+          <t>25479797</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Emma</t>
+          <t>"Mohamed Alnaqbi"</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -2954,14 +2954,14 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>3848</t>
+          <t>3930</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>27161</t>
+          <t>26616</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -2981,14 +2981,14 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>3701</t>
+          <t>3851</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>28166</t>
+          <t>28872</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -3008,14 +3008,14 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>3655</t>
+          <t>3741</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>30800</t>
+          <t>30779</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -3035,14 +3035,14 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>3543</t>
+          <t>3657</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>57008</t>
+          <t>47505</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -3062,7 +3062,7 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>2606</t>
+          <t>2943</t>
         </is>
       </c>
     </row>
@@ -3096,7 +3096,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>17306</t>
+          <t>15659</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -3116,14 +3116,14 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>4222</t>
+          <t>4485</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>27363</t>
+          <t>24951</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -3143,14 +3143,14 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>3693</t>
+          <t>3941</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>29388</t>
+          <t>29244</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -3170,14 +3170,14 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>3601</t>
+          <t>3723</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>30768</t>
+          <t>30659</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -3197,24 +3197,24 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>3544</t>
+          <t>3662</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>32879</t>
+          <t>32595</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>47459684</t>
+          <t>55634661</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>㊥阿闹切克闹</t>
+          <t>Opalus</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -3224,24 +3224,24 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>3456</t>
+          <t>3576</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>34106</t>
+          <t>32965</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>55634661</t>
+          <t>47459684</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Opalus</t>
+          <t>㊥阿闹切克闹</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -3251,24 +3251,24 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>3406</t>
+          <t>3560</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>36208</t>
+          <t>37111</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>56379103</t>
+          <t>56585361</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>Globalking</t>
+          <t>"㊥ go策划我要ali"</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -3278,14 +3278,14 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>3322</t>
+          <t>3380</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>36356</t>
+          <t>37589</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -3305,24 +3305,24 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>3316</t>
+          <t>3359</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>37482</t>
+          <t>38182</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>56732705</t>
+          <t>56379103</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>时间温柔皆遗憾</t>
+          <t>Globalking</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -3332,24 +3332,24 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>3271</t>
+          <t>3335</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>38183</t>
+          <t>39472</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>3391765</t>
+          <t>47430231</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>马er</t>
+          <t>Kentantrino</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -3359,24 +3359,24 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>3244</t>
+          <t>3281</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>39766</t>
+          <t>40110</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>56585361</t>
+          <t>56732705</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>"㊥ go策划我要ali"</t>
+          <t>时间温柔皆遗憾</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -3386,24 +3386,24 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>3183</t>
+          <t>3254</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>44364</t>
+          <t>40240</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>58743790</t>
+          <t>3391765</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Ma</t>
+          <t>马er</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -3413,24 +3413,24 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>2999</t>
+          <t>3249</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>44905</t>
+          <t>41106</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>48634530</t>
+          <t>47244896</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>leezhenrui</t>
+          <t>Dropthebeat</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -3440,24 +3440,24 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>2980</t>
+          <t>3216</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>45502</t>
+          <t>43152</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>47244896</t>
+          <t>58743790</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Dropthebeat</t>
+          <t>Ma</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -3467,24 +3467,24 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>2957</t>
+          <t>3126</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>46008</t>
+          <t>44180</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>47430231</t>
+          <t>11645391</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Kentantrino</t>
+          <t>"omar omar"</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -3494,24 +3494,24 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>2938</t>
+          <t>3082</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>46468</t>
+          <t>44433</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>58839983</t>
+          <t>48634530</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>青龙偃月灯</t>
+          <t>leezhenrui</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -3521,14 +3521,14 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>2921</t>
+          <t>3072</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>47408</t>
+          <t>45836</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -3548,24 +3548,24 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>2889</t>
+          <t>3012</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>50515</t>
+          <t>46950</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>20372140</t>
+          <t>58839983</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>人山即是仙</t>
+          <t>青龙偃月灯</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -3575,24 +3575,24 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>2782</t>
+          <t>2966</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>50893</t>
+          <t>51913</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>58641574</t>
+          <t>20372140</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Player-58641574鱼</t>
+          <t>人山即是仙</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -3602,24 +3602,24 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>2769</t>
+          <t>2782</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>54829</t>
+          <t>52380</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>1304123</t>
+          <t>58641574</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Cccccccccccc</t>
+          <t>Player-58641574鱼</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -3629,14 +3629,14 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>2659</t>
+          <t>2766</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>56622</t>
+          <t>56240</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -3656,24 +3656,24 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>2614</t>
+          <t>2656</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>58066</t>
+          <t>57754</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>11645391</t>
+          <t>1304123</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>"omar omar"</t>
+          <t>Cccccccccccc</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -3683,14 +3683,14 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>2585</t>
+          <t>2619</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>58827</t>
+          <t>59936</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -3710,14 +3710,14 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>2570</t>
+          <t>2572</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>59882</t>
+          <t>61154</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -3737,24 +3737,24 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>2550</t>
+          <t>2548</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>61431</t>
+          <t>62680</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>5367482</t>
+          <t>43281368</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Ігор</t>
+          <t>xhs2763</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
@@ -3764,24 +3764,24 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>2523</t>
+          <t>2522</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>62812</t>
+          <t>62963</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>43281368</t>
+          <t>5367482</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>xhs2763</t>
+          <t>Ігор</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
@@ -3791,14 +3791,14 @@
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>2502</t>
+          <t>2517</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>70220</t>
+          <t>71230</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3818,14 +3818,14 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>2352</t>
+          <t>2351</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>70904</t>
+          <t>72419</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3845,7 +3845,7 @@
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>2333</t>
+          <t>2317</t>
         </is>
       </c>
     </row>
@@ -4014,7 +4014,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>50235</t>
+          <t>48571</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -4034,14 +4034,14 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>2791</t>
+          <t>2901</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>47137</t>
+          <t>45815</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -4061,14 +4061,14 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>2898</t>
+          <t>3013</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>54095</t>
+          <t>54748</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -4088,14 +4088,14 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>2677</t>
+          <t>2698</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>62992</t>
+          <t>62096</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
@@ -4115,14 +4115,14 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>2500</t>
+          <t>2531</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>67622</t>
+          <t>69070</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -4142,14 +4142,14 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>2421</t>
+          <t>2409</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>78063</t>
+          <t>77869</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -4169,14 +4169,14 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>2173</t>
+          <t>2197</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>110360</t>
+          <t>112907</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -4196,14 +4196,14 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>1514</t>
+          <t>1506</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>232088</t>
+          <t>241131</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -4230,7 +4230,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>9598</t>
+          <t>6988</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -4250,14 +4250,14 @@
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>4785</t>
+          <t>5270</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>24166</t>
+          <t>26643</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
@@ -4284,7 +4284,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>53441</t>
+          <t>52048</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
@@ -4304,14 +4304,14 @@
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>2694</t>
+          <t>2777</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>62239</t>
+          <t>63337</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -4446,7 +4446,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>55914</t>
+          <t>55707</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4466,7 +4466,7 @@
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>2632</t>
+          <t>2670</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 24-01-13 11:31:18
</commit_message>
<xml_diff>
--- a/Season_Trophies/84.xlsx
+++ b/Season_Trophies/84.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E154"/>
+  <dimension ref="A1:E158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2799,17 +2799,17 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3391</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>1222440</t>
+          <t>1673125</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>"Sneaky Ninja Panda"</t>
+          <t>"birrkoff1 ᴿᴵᴾ"</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -2819,24 +2819,24 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>6575</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>62830</t>
+          <t>2915</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>1304123</t>
+          <t>2380957</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Cccccccccccc</t>
+          <t>"ᴱᵁᴿ Biggymike ᶰᶫ"</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -2846,24 +2846,24 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>2562</t>
+          <t>6679</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>43524</t>
+          <t>2031</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>3391765</t>
+          <t>3165166</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>马er</t>
+          <t>EurPapaStressato</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -2873,24 +2873,24 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>3284</t>
+          <t>6904</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>33053</t>
+          <t>4663</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>3649043</t>
+          <t>4388412</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>"慶頴 謝"</t>
+          <t>"RIP 12ThSt NXS"</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -2900,24 +2900,24 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>3798</t>
+          <t>6349</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>62012</t>
+          <t>2676</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>5367482</t>
+          <t>4705659</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Ігор</t>
+          <t>"EUR Broken Arrow"</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -2927,24 +2927,24 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>2578</t>
+          <t>6745</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>31842</t>
+          <t>2036</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>9718882</t>
+          <t>4977474</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>小霸王2021</t>
+          <t>Wisam2112</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -2954,24 +2954,24 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>3853</t>
+          <t>6897</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>47051</t>
+          <t>1896</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>11645391</t>
+          <t>5093883</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>"omar omar"</t>
+          <t>"Galadriel ᴱᵁᴿ"</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -2981,24 +2981,24 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>3108</t>
+          <t>6930</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>4017</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>15436348</t>
+          <t>5389668</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Lucas</t>
+          <t>"Alvils ᴱᵁᴿ"</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -3008,24 +3008,24 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>6460</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>26599</t>
+          <t>2654</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>18082891</t>
+          <t>5644133</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>"SilverHawk EUR"</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -3035,24 +3035,24 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>4113</t>
+          <t>6745</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>52296</t>
+          <t>5452</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>20372140</t>
+          <t>6087115</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>人山即是仙</t>
+          <t>"King Salomon ️"</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -3062,24 +3062,24 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>2869</t>
+          <t>6198</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>16085</t>
+          <t>3526</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>25163202</t>
+          <t>6179013</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>"sam yang"</t>
+          <t>"रहमत      सरकार"</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -3089,24 +3089,24 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>4817</t>
+          <t>6559</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>24876</t>
+          <t>3467</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>25479797</t>
+          <t>7350052</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>"Mohamed Alnaqbi"</t>
+          <t>kummituskäedᴱᵁᴿ</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -3116,24 +3116,24 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>4227</t>
+          <t>6567</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>31152</t>
+          <t>2670</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>28855852</t>
+          <t>7488623</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>tiger</t>
+          <t>"RAGNARⁿ ╳ ˢ"</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -3143,24 +3143,24 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>3884</t>
+          <t>6738</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>17207</t>
+          <t>1596</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>31134300</t>
+          <t>8223979</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>McMaX</t>
+          <t>Lastangryman</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -3170,24 +3170,24 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>4732</t>
+          <t>7008</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>21673</t>
+          <t>2077</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>37069173</t>
+          <t>8658951</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>詹toniii</t>
+          <t>"EUR gabriele  b"</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -3197,24 +3197,24 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>4481</t>
+          <t>6881</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3216</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>38994054</t>
+          <t>9161108</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>chengnan</t>
+          <t>"ᴱᵁᴿ Rankos ᶰᶫ"</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -3224,24 +3224,24 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>6618</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>63268</t>
+          <t>2909</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>43281368</t>
+          <t>9178517</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>xhs2763</t>
+          <t>"julo2000 AOW"</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -3251,24 +3251,24 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>2553</t>
+          <t>6692</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2196</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>44378757</t>
+          <t>9730363</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>"NᵉᵗʰᵉʳDʳⁱᶠᵗᵉʳ ㊥"</t>
+          <t>EURythmics</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -3278,24 +3278,24 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>6863</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>26262</t>
+          <t>2006</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>44708798</t>
+          <t>10148497</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>"㊥ mythgod"</t>
+          <t>Cobraⁿˣˢ</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -3305,24 +3305,24 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>4134</t>
+          <t>6909</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>33608</t>
+          <t>3258</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>46289694</t>
+          <t>10960737</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>㊥Vincent</t>
+          <t>"Klebsiella P"</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -3332,24 +3332,24 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>3767</t>
+          <t>6584</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>54086</t>
+          <t>1705</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>47227626</t>
+          <t>11511350</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>Player-47227626</t>
+          <t>"Perrin Aybara"</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -3359,24 +3359,24 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>2803</t>
+          <t>6971</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>33663</t>
+          <t>4271</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>47244896</t>
+          <t>12011386</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Dropthebeat</t>
+          <t>"NXS4  paulosilva"</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -3386,24 +3386,24 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>3764</t>
+          <t>6420</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>38508</t>
+          <t>3607</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>47430231</t>
+          <t>13102210</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Kentantrino</t>
+          <t>SirBearⱽᴱᶜᴼᴳEUR</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -3413,24 +3413,24 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>3505</t>
+          <t>6542</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>34751</t>
+          <t>3913</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>47459684</t>
+          <t>13589486</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>㊥阿闹切克闹</t>
+          <t>"EUR vytelis"</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -3440,24 +3440,24 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>3700</t>
+          <t>6469</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>43134</t>
+          <t>2798</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>48634530</t>
+          <t>13602346</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>leezhenrui</t>
+          <t>"EUR•Kungfu Jesus"</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -3467,24 +3467,24 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>3301</t>
+          <t>6719</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>75168</t>
+          <t>3643</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>52792063</t>
+          <t>13957661</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>"Tramaine Dowlen"</t>
+          <t>"ᴱᵁᴿ MIROZ ᴵᵀᴬ"</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -3494,24 +3494,24 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>2306</t>
+          <t>6537</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>40180</t>
+          <t>3081</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>52997727</t>
+          <t>15409989</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>larios</t>
+          <t>"WarDan ⁿ ╳ ˢ EUR"</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -3521,24 +3521,24 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>3427</t>
+          <t>6654</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>29962</t>
+          <t>2945</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>54085771</t>
+          <t>15934629</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>㊥Matthieu</t>
+          <t>"ᴿᴵᴾStingray ᴱᵁᴿ"</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -3548,24 +3548,24 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>3939</t>
+          <t>6684</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2557</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>54588689</t>
+          <t>16334976</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>㊥墨衍枫迹☜</t>
+          <t>"vanneurk - EUR"</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -3575,24 +3575,24 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>6778</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>23229</t>
+          <t>9999</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>54778421</t>
+          <t>16723167</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Emma</t>
+          <t>Misza</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -3602,24 +3602,24 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>4345</t>
+          <t>5673</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>63391</t>
+          <t>2486</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>55499394</t>
+          <t>18899977</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Player-55499394</t>
+          <t>"Dusan MNE"</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -3629,24 +3629,24 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>2550</t>
+          <t>6704</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>30307</t>
+          <t>3578</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>55634661</t>
+          <t>19074651</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Opalus</t>
+          <t>"EUR ThugLife ⁠ "</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
@@ -3656,24 +3656,24 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>3920</t>
+          <t>6536</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1293</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>55810157</t>
+          <t>20040315</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Beard</t>
+          <t>ᴱᵁᴿMethadataᴿᴵᴾ</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -3683,24 +3683,24 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>7104</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>37316</t>
+          <t>3126</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>56379103</t>
+          <t>21518036</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Globalking</t>
+          <t>"Eᑌᖇ ᒪᔕᗪ TᖇIᑭ"</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
@@ -3710,24 +3710,24 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>3564</t>
+          <t>6644</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>39405</t>
+          <t>3057</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>56585361</t>
+          <t>22018497</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>"㊥ go策划我要ali"</t>
+          <t>"conway EUR"</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -3737,24 +3737,24 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>3463</t>
+          <t>6659</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>31772</t>
+          <t>2590</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>56700848</t>
+          <t>23803177</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>工口漫画老师</t>
+          <t>"Stain  SIT  Tha"</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
@@ -3764,24 +3764,24 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>3856</t>
+          <t>6767</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>38217</t>
+          <t>4046</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>56732705</t>
+          <t>25045159</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>时间温柔皆遗憾</t>
+          <t>"EUR marius army"</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
@@ -3791,24 +3791,24 @@
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>3517</t>
+          <t>6459</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>73959</t>
+          <t>3087</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>57219176</t>
+          <t>25735452</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>青莲道人</t>
+          <t>"Tanvir nxs"</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
@@ -3818,24 +3818,24 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>2336</t>
+          <t>6641</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1590</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>57556179</t>
+          <t>26012001</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>特战新生代英雄</t>
+          <t>"OlivaFritta ᴱᵁᴿ"</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
@@ -3845,24 +3845,24 @@
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>6995</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>839</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>58340439</t>
+          <t>26910302</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>70qilin</t>
+          <t>"ᴱᵁᴿ Caribrain ᶰᶫ"</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -3872,24 +3872,24 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>7258</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>48417</t>
+          <t>2641</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>58408326</t>
+          <t>27402692</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>"Killer Bee"</t>
+          <t>"Vec Fontaine"</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
@@ -3899,24 +3899,24 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>3037</t>
+          <t>6755</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>61576</t>
+          <t>2462</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>58615925</t>
+          <t>27636303</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>齐天的大圣</t>
+          <t>ᴱᵁᴿStressatoᴵᵀᴬ</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
@@ -3926,24 +3926,24 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>2586</t>
+          <t>6801</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>53526</t>
+          <t>3846</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>58641574</t>
+          <t>31723587</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>Player-58641574鱼</t>
+          <t>"Hussain VEC"</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
@@ -3953,24 +3953,24 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>2822</t>
+          <t>6490</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>44796</t>
+          <t>2012</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>58743790</t>
+          <t>36057737</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Ma</t>
+          <t>ᴿᴵᴾObliterateᴱᵁᴿ</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
@@ -3980,24 +3980,24 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>3226</t>
+          <t>6909</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>46991</t>
+          <t>3539</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>58839983</t>
+          <t>38867140</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>每逢佳节胖六斤</t>
+          <t>"EUR harleyjoebob"</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
@@ -4007,132 +4007,132 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>3110</t>
+          <t>6549</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2977</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>29355299</t>
+          <t>39060442</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>Player-29355299</t>
+          <t>"Ronny Yen  ⁿ ╳ ˢ"</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>6676</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>50646</t>
+          <t>4766</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>41849539</t>
+          <t>45410553</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>三号馆馆主</t>
+          <t>Niero</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>2935</t>
+          <t>6308</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>58054</t>
+          <t>1713</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>47622456</t>
+          <t>47772380</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>伊恩</t>
+          <t>"EUR FeistyPickle"</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>2676</t>
+          <t>6978</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>63115</t>
+          <t>2989</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>49553719</t>
+          <t>54409793</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>"Oreo Captain Sir"</t>
+          <t>Bare_North</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>2556</t>
+          <t>6651</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>70263</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>55210350</t>
+          <t>29355299</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>一个过客而已</t>
+          <t>Player-29355299</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
@@ -4142,24 +4142,24 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>2432</t>
+          <t>1000</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>50646</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>55745105</t>
+          <t>41849539</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>eldeniz</t>
+          <t>三号馆馆主</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
@@ -4169,24 +4169,24 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>1438</t>
+          <t>2935</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>45940</t>
+          <t>58054</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>56241637</t>
+          <t>47622456</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>Player-14day</t>
+          <t>伊恩</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
@@ -4196,24 +4196,24 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>3167</t>
+          <t>2676</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>75264</t>
+          <t>63115</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>58572199</t>
+          <t>49553719</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>你干嘛～哎呦～</t>
+          <t>"Oreo Captain Sir"</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
@@ -4223,24 +4223,24 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>2303</t>
+          <t>2556</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>70263</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>58766144</t>
+          <t>55210350</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>EquablePrecedence38</t>
+          <t>一个过客而已</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
@@ -4250,7 +4250,7 @@
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>1524</t>
+          <t>2432</t>
         </is>
       </c>
     </row>
@@ -4262,12 +4262,12 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>58910668</t>
+          <t>55745105</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>BrittleAuthor33</t>
+          <t>eldeniz</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
@@ -4277,132 +4277,132 @@
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>1027</t>
+          <t>1438</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>31946</t>
+          <t>45940</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>6010122</t>
+          <t>56241637</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>"Edward Peng"</t>
+          <t>Player-14day</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>Chinese</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>3849</t>
+          <t>3167</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>75264</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>8850180</t>
+          <t>58572199</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>30624300</t>
+          <t>你干嘛～哎呦～</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>Chinese</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2303</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>65570</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>9195340</t>
+          <t>58766144</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>Namllllllik</t>
+          <t>EquablePrecedence38</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>Chinese</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>2511</t>
+          <t>1524</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>6192</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>9913517</t>
+          <t>58910668</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>"Kenny Chan"</t>
+          <t>BrittleAuthor33</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>Chinese</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>6052</t>
+          <t>1027</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>53599</t>
+          <t>31946</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>10636651</t>
+          <t>6010122</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>"Ismail Aflou"</t>
+          <t>"Edward Peng"</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
@@ -4412,7 +4412,7 @@
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>2820</t>
+          <t>3849</t>
         </is>
       </c>
     </row>
@@ -4424,12 +4424,12 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>12648101</t>
+          <t>8850180</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>"player 198827"</t>
+          <t>30624300</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
@@ -4446,17 +4446,17 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>65570</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>15755724</t>
+          <t>9195340</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>"Last Good"</t>
+          <t>Namllllllik</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
@@ -4466,24 +4466,24 @@
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2511</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>6192</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>28624723</t>
+          <t>9913517</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>"Woody Shade"</t>
+          <t>"Kenny Chan"</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
@@ -4493,32 +4493,140 @@
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>6052</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
+          <t>53599</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>10636651</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>"Ismail Aflou"</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>2820</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>12648101</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>"player 198827"</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>15755724</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>"Last Good"</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>28624723</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>"Woody Shade"</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
           <t>51089</t>
         </is>
       </c>
-      <c r="B154" t="inlineStr">
+      <c r="B158" t="inlineStr">
         <is>
           <t>41848598</t>
         </is>
       </c>
-      <c r="C154" t="inlineStr">
+      <c r="C158" t="inlineStr">
         <is>
           <t>国家一级保护沙雕</t>
         </is>
       </c>
-      <c r="D154" t="inlineStr">
+      <c r="D158" t="inlineStr">
         <is>
           <t>Chinese</t>
         </is>
       </c>
-      <c r="E154" t="inlineStr">
+      <c r="E158" t="inlineStr">
         <is>
           <t>2917</t>
         </is>

</xml_diff>